<commit_message>
Updated Release schedule in Use case sheet
</commit_message>
<xml_diff>
--- a/Project Reference Data.xlsx
+++ b/Project Reference Data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
   <si>
     <t>System</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t>View landing page</t>
   </si>
   <si>
     <t>View product list in a category</t>
@@ -634,6 +631,39 @@
 API &amp; Data queries:
 POST /customers/{id}/addresses
 &lt;address&gt;</t>
+  </si>
+  <si>
+    <t>Release Target</t>
+  </si>
+  <si>
+    <t>R1.0</t>
+  </si>
+  <si>
+    <t>View categories on home page</t>
+  </si>
+  <si>
+    <t>View home page</t>
+  </si>
+  <si>
+    <t>View banners</t>
+  </si>
+  <si>
+    <t>View 'products on offer' listing scroll</t>
+  </si>
+  <si>
+    <t>View 'recent upload product' listing scroll</t>
+  </si>
+  <si>
+    <t>Search for a product</t>
+  </si>
+  <si>
+    <t>View related products listing scroll</t>
+  </si>
+  <si>
+    <t>View membership info</t>
+  </si>
+  <si>
+    <t>Can customer purchase from app?</t>
   </si>
 </sst>
 </file>
@@ -987,21 +1017,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1041,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1019,7 +1050,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1028,12 +1059,12 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1041,911 +1072,1080 @@
         <v>7</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H5" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C7" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C8" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C10" s="3" t="s">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C12" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="H12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
-      <c r="C17" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-      <c r="C18" s="13" t="s">
-        <v>103</v>
+      <c r="C17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19">
+        <v>88</v>
+      </c>
+      <c r="H18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G20" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B21" s="3"/>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
-      <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="H22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
-      <c r="C23" s="2" t="s">
-        <v>17</v>
+      <c r="C23" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
-        <v>18</v>
+        <v>88</v>
+      </c>
+      <c r="H23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+      <c r="C24" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="3"/>
-      <c r="C25" s="2" t="s">
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="H24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-      <c r="C26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="H25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="H26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>22</v>
+        <v>88</v>
+      </c>
+      <c r="H27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B29" s="3" t="s">
-        <v>23</v>
+        <v>88</v>
+      </c>
+      <c r="H28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+      <c r="C29" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B30" s="12" t="s">
-        <v>115</v>
+        <v>88</v>
+      </c>
+      <c r="H29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C31" s="12" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="H30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B31" s="3"/>
+      <c r="C31" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="3" t="s">
-        <v>24</v>
+        <v>88</v>
+      </c>
+      <c r="H31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
+      <c r="C32" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="11" t="s">
-        <v>113</v>
+        <v>88</v>
+      </c>
+      <c r="H32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="3"/>
+      <c r="C33" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E33">
         <v>2</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C34" s="12" t="s">
-        <v>110</v>
+        <v>88</v>
+      </c>
+      <c r="H33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C35" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E35">
+      <c r="G36" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C37" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37">
         <v>1</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C36" s="3" t="s">
+      <c r="G37" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C39" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C40" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C41" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="11"/>
+      <c r="H46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B39" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B42" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B43" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B44" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B45" s="3" t="s">
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B46" s="3" t="s">
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47">
-        <v>3</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B48" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48">
-        <v>3</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B49" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49">
-        <v>3</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B50" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50">
-        <v>3</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B51" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E51">
-        <v>3</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B52" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B53" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E53">
-        <v>3</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B54" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E54">
         <v>3</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="H54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E55">
         <v>3</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="H55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E56">
         <v>3</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="3" t="s">
-        <v>59</v>
+        <v>88</v>
+      </c>
+      <c r="H56" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="E57">
         <v>3</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="3" t="s">
-        <v>58</v>
+        <v>88</v>
+      </c>
+      <c r="H57" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B58" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="H58" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E59">
         <v>3</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="E60">
         <v>3</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="E61">
         <v>3</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" t="s">
+        <v>141</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B70" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B71" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-    </row>
-    <row r="63" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B63" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63">
+      <c r="E71">
         <v>1</v>
       </c>
-      <c r="G63" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B64" s="2" t="s">
+      <c r="G71" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B72" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B65" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B67" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E67">
-        <v>2</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B68" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C69" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C70" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E70">
-        <v>2</v>
-      </c>
-      <c r="G70" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B71" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E71">
-        <v>2</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="E72">
         <v>1</v>
       </c>
       <c r="G72" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" t="s">
-        <v>69</v>
+      <c r="B73" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G73" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
+      <c r="B74" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="75" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
+      <c r="B75" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C76" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" t="s">
+        <v>68</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="8" t="s">
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+    </row>
+    <row r="84" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="9"/>
+      <c r="B84" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-    </row>
-    <row r="77" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="9"/>
-      <c r="B77" s="8" t="s">
+      <c r="C84" s="9"/>
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="9"/>
+      <c r="B85" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C77" s="9"/>
-      <c r="G77" s="3"/>
-    </row>
-    <row r="78" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
-      <c r="B78" s="8" t="s">
+      <c r="C85" s="9"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="9"/>
+      <c r="B86" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="9"/>
-      <c r="B79" s="8" t="s">
+      <c r="C86" s="9"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="9"/>
+      <c r="B87" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C79" s="9"/>
-      <c r="G79" s="3"/>
-    </row>
-    <row r="80" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="9"/>
-      <c r="B80" s="8" t="s">
+      <c r="C87" s="9"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="9"/>
+      <c r="B88" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="9"/>
-      <c r="G80" s="3"/>
-    </row>
-    <row r="81" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="9"/>
-      <c r="B81" s="8" t="s">
+      <c r="C88" s="9"/>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="9"/>
+      <c r="B89" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C81" s="9"/>
-      <c r="G81" s="3"/>
-    </row>
-    <row r="82" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="9"/>
-      <c r="B82" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C82" s="9"/>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="C89" s="9"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>80</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B103" s="13" t="s">
+      <c r="B103" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B111" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="13" t="s">
+    <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B112" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="13" t="s">
+    <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="13"/>
-    </row>
-    <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="13"/>
-    </row>
-    <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="13"/>
+    <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="13"/>
+    </row>
+    <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B115" s="13"/>
+    </row>
+    <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B116" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1970,164 +2170,164 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>85</v>
-      </c>
       <c r="D1" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="D3" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="344.25" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2177,7 +2377,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>